<commit_message>
ADC now working; To be done: showing it to the lcd
</commit_message>
<xml_diff>
--- a/TouchGFX/assets/texts/texts.xlsx
+++ b/TouchGFX/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3212" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4523" uniqueCount="112">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -270,6 +270,88 @@
   </si>
   <si>
     <t xml:space="preserve">Codemaze - TGFX sample application</t>
+  </si>
+  <si>
+    <t xml:space="preserve">New Text&lt;value&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">New Text&lt;value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ADC </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ADC value = </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ADC value = &lt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ADC value = &lt;value&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ADC value = &lt;value&gt;V</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0-1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0-8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3.3V</t>
+  </si>
+  <si>
+    <t xml:space="preserve">.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C</t>
+  </si>
+  <si>
+    <t xml:space="preserve">N</t>
+  </si>
+  <si>
+    <t xml:space="preserve">New ADC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">New ADC </t>
+  </si>
+  <si>
+    <t xml:space="preserve">New ADC m</t>
+  </si>
+  <si>
+    <t xml:space="preserve">New ADC measure</t>
+  </si>
+  <si>
+    <t xml:space="preserve">New ADC measur</t>
+  </si>
+  <si>
+    <t xml:space="preserve">New AD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10</t>
   </si>
 </sst>
 </file>
@@ -1495,8 +1577,12 @@
       <c r="F4" t="s">
         <v>17</v>
       </c>
-      <c r="G4"/>
-      <c r="H4"/>
+      <c r="G4" t="s">
+        <v>52</v>
+      </c>
+      <c r="H4" t="s">
+        <v>52</v>
+      </c>
       <c r="I4"/>
       <c r="K4" s="4" t="s">
         <v>9</v>
@@ -1735,9 +1821,57 @@
         <v>36</v>
       </c>
     </row>
-    <row r="4"/>
-    <row r="5"/>
-    <row r="6"/>
+    <row r="4">
+      <c r="B4" t="s">
+        <v>41</v>
+      </c>
+      <c r="C4" t="s">
+        <v>37</v>
+      </c>
+      <c r="D4" t="s">
+        <v>42</v>
+      </c>
+      <c r="E4" t="s">
+        <v>43</v>
+      </c>
+      <c r="F4" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="B5" t="s">
+        <v>48</v>
+      </c>
+      <c r="C5" t="s">
+        <v>37</v>
+      </c>
+      <c r="D5" t="s">
+        <v>42</v>
+      </c>
+      <c r="E5" t="s">
+        <v>43</v>
+      </c>
+      <c r="F5" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="B6" t="s">
+        <v>55</v>
+      </c>
+      <c r="C6" t="s">
+        <v>37</v>
+      </c>
+      <c r="D6" t="s">
+        <v>50</v>
+      </c>
+      <c r="E6" t="s">
+        <v>43</v>
+      </c>
+      <c r="F6" t="s">
+        <v>103</v>
+      </c>
+    </row>
     <row r="7"/>
     <row r="8"/>
     <row r="9"/>

</xml_diff>

<commit_message>
ADC is shown on the LCD. The output is wrong though. Only 3 digits are shown.
</commit_message>
<xml_diff>
--- a/TouchGFX/assets/texts/texts.xlsx
+++ b/TouchGFX/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4523" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4637" uniqueCount="114">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -352,6 +352,12 @@
   </si>
   <si>
     <t xml:space="preserve">10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">100</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1000</t>
   </si>
 </sst>
 </file>
@@ -1852,26 +1858,10 @@
         <v>43</v>
       </c>
       <c r="F5" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
     </row>
-    <row r="6">
-      <c r="B6" t="s">
-        <v>55</v>
-      </c>
-      <c r="C6" t="s">
-        <v>37</v>
-      </c>
-      <c r="D6" t="s">
-        <v>50</v>
-      </c>
-      <c r="E6" t="s">
-        <v>43</v>
-      </c>
-      <c r="F6" t="s">
-        <v>103</v>
-      </c>
-    </row>
+    <row r="6"/>
     <row r="7"/>
     <row r="8"/>
     <row r="9"/>

</xml_diff>

<commit_message>
D3 Pin's current voltage level is printed to the LCD via ADC.
</commit_message>
<xml_diff>
--- a/TouchGFX/assets/texts/texts.xlsx
+++ b/TouchGFX/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4637" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4977" uniqueCount="120">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -358,6 +358,24 @@
   </si>
   <si>
     <t xml:space="preserve">1000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3.30</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3.301</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ADC value = &lt;value&gt;v</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0-4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0-40</t>
   </si>
 </sst>
 </file>
@@ -1584,7 +1602,7 @@
         <v>17</v>
       </c>
       <c r="G4" t="s">
-        <v>52</v>
+        <v>98</v>
       </c>
       <c r="H4" t="s">
         <v>52</v>
@@ -1841,7 +1859,7 @@
         <v>43</v>
       </c>
       <c r="F4" t="s">
-        <v>91</v>
+        <v>117</v>
       </c>
     </row>
     <row r="5">
@@ -1858,7 +1876,7 @@
         <v>43</v>
       </c>
       <c r="F5" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
     </row>
     <row r="6"/>

</xml_diff>

<commit_message>
Add labels to the graph
</commit_message>
<xml_diff>
--- a/TouchGFX/assets/texts/texts.xlsx
+++ b/TouchGFX/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5162" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8590" uniqueCount="135">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -315,6 +315,111 @@
   </si>
   <si>
     <t xml:space="preserve">V4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">t [ms]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3.0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">t[ms]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[ms]</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> [Hz]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[Hz]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[kHz]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3.2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2New Text</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2.New Text</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2.4New Text</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2.4ew Text</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2.4ext</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2.4xt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2.4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2.5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">New </t>
+  </si>
+  <si>
+    <t xml:space="preserve">7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7.6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7.5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId13</t>
+  </si>
+  <si>
+    <t xml:space="preserve">New Tex</t>
   </si>
 </sst>
 </file>
@@ -1794,7 +1899,7 @@
         <v>43</v>
       </c>
       <c r="F4" t="s">
-        <v>85</v>
+        <v>108</v>
       </c>
     </row>
     <row r="5">
@@ -1811,7 +1916,7 @@
         <v>43</v>
       </c>
       <c r="F5" t="s">
-        <v>86</v>
+        <v>105</v>
       </c>
     </row>
     <row r="6">
@@ -1862,7 +1967,7 @@
         <v>43</v>
       </c>
       <c r="F8" t="s">
-        <v>91</v>
+        <v>109</v>
       </c>
     </row>
     <row r="9">
@@ -1879,7 +1984,7 @@
         <v>43</v>
       </c>
       <c r="F9" t="s">
-        <v>92</v>
+        <v>112</v>
       </c>
     </row>
     <row r="10">
@@ -1896,7 +2001,7 @@
         <v>43</v>
       </c>
       <c r="F10" t="s">
-        <v>97</v>
+        <v>127</v>
       </c>
     </row>
     <row r="11">
@@ -1913,9 +2018,78 @@
         <v>43</v>
       </c>
       <c r="F11" t="s">
-        <v>99</v>
-      </c>
-    </row>
+        <v>111</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="B12" t="s">
+        <v>113</v>
+      </c>
+      <c r="C12" t="s">
+        <v>37</v>
+      </c>
+      <c r="D12" t="s">
+        <v>42</v>
+      </c>
+      <c r="E12" t="s">
+        <v>43</v>
+      </c>
+      <c r="F12" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="B13" t="s">
+        <v>115</v>
+      </c>
+      <c r="C13" t="s">
+        <v>37</v>
+      </c>
+      <c r="D13" t="s">
+        <v>42</v>
+      </c>
+      <c r="E13" t="s">
+        <v>43</v>
+      </c>
+      <c r="F13" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="B14" t="s">
+        <v>123</v>
+      </c>
+      <c r="C14" t="s">
+        <v>37</v>
+      </c>
+      <c r="D14" t="s">
+        <v>42</v>
+      </c>
+      <c r="E14" t="s">
+        <v>43</v>
+      </c>
+      <c r="F14" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="B15" t="s">
+        <v>124</v>
+      </c>
+      <c r="C15" t="s">
+        <v>37</v>
+      </c>
+      <c r="D15" t="s">
+        <v>42</v>
+      </c>
+      <c r="E15" t="s">
+        <v>43</v>
+      </c>
+      <c r="F15" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="16"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B2:E2"/>

</xml_diff>